<commit_message>
trajectory returns discounted reward, auc, docs
</commit_message>
<xml_diff>
--- a/hieu/scratch.xlsx
+++ b/hieu/scratch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hihoan\local\workspace\github\IncrementalMining\hieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B5EDA2-FB19-4641-BBB7-B3CB9C5A444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA60938-DB13-4E4A-99C4-9EFB6F6A94D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>#iter</t>
+  </si>
+  <si>
+    <t>gp</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -88,36 +102,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -127,6 +111,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -151,10 +146,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$12</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -183,12 +178,15 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>500</c:v>
                 </c:pt>
               </c:numCache>
@@ -196,10 +194,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$12</c:f>
+              <c:f>Sheet1!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>57342</c:v>
                 </c:pt>
@@ -226,6 +224,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>60603</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -234,6 +235,121 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DE26-4EE9-8229-B67EB52BC9CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dummy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>55677</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55369</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56197</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5F22-48C4-BD53-B77CC6E56C08}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -380,6 +496,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -984,16 +1131,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>102393</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>564356</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>140493</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>602456</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1284,98 +1431,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:C12"/>
+  <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B1">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B2">
         <v>5</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>57342</v>
       </c>
+      <c r="D2">
+        <v>55677</v>
+      </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B3">
         <v>10</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>57432</v>
       </c>
+      <c r="D3">
+        <v>57505</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B4">
         <v>20</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>57555</v>
       </c>
+      <c r="D4">
+        <v>55369</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B5">
         <v>30</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>57039</v>
       </c>
+      <c r="D5">
+        <v>56197</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B6">
         <v>40</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>60240</v>
       </c>
+      <c r="D6">
+        <v>56063</v>
+      </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B7">
         <v>50</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>55997</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8">
         <v>100</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>56856</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9">
         <v>150</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>61229</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B9">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10">
         <v>200</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>60603</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>250</v>
+      </c>
+      <c r="C11">
+        <v>59456</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B12">
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13">
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B14">
         <v>500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
train with multiple domains
</commit_message>
<xml_diff>
--- a/hieu/scratch.xlsx
+++ b/hieu/scratch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hihoan\local\workspace\github\IncrementalMining\hieu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520258D6-6F95-4069-94F8-276C015C47C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49FA787-094A-45A1-85D9-BA058BF05DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.104580927384077"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.85752580927384092"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -227,6 +237,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>59456</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -501,6 +514,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.83944006999125109"/>
+          <c:y val="0.72280037911927697"/>
+          <c:w val="0.12167104111986002"/>
+          <c:h val="0.15625109361329834"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1437,7 +1460,7 @@
   <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1555,6 +1578,9 @@
       <c r="B12">
         <v>300</v>
       </c>
+      <c r="C12">
+        <v>61039</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13">

</xml_diff>